<commit_message>
add all output files to docs folder for github pages
</commit_message>
<xml_diff>
--- a/docs/all-profiles.xlsx
+++ b/docs/all-profiles.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1609" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2710" uniqueCount="413">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-10-30T14:42:12-04:00</t>
+    <t>2024-10-31T11:09:52-04:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -969,6 +969,342 @@
   </si>
   <si>
     <t>http://hl7.org/fhir/ValueSet/link-type|4.0.1</t>
+  </si>
+  <si>
+    <t>digicert-group-profile</t>
+  </si>
+  <si>
+    <t>http://example.org/StructureDefinition/digicert-group-profile</t>
+  </si>
+  <si>
+    <t>DigiCertGroup</t>
+  </si>
+  <si>
+    <t>Digital Cert FHIR Bulk Group Profile</t>
+  </si>
+  <si>
+    <t>This is a group profile used in FHIR export Operation to obtain a detailed set of FHIR resources of diverse resource types pertaining to all members of the Group</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/StructureDefinition/Group</t>
+  </si>
+  <si>
+    <t>Group of multiple entities</t>
+  </si>
+  <si>
+    <t>Represents a defined collection of entities that may be discussed or acted upon collectively but which are not expected to act collectively, and are not formally or legally recognized; i.e. a collection of entities that isn't an Organization.</t>
+  </si>
+  <si>
+    <t>If both Group.characteristic and Group.member are present, then the members are the individuals who were found who met the characteristic.  It's possible that there might be other candidate members who meet the characteristic and aren't (yet) in the list.  All members SHALL have the listed characteristics.</t>
+  </si>
+  <si>
+    <t>dom-2:If the resource is contained in another resource, it SHALL NOT contain nested Resources {contained.contained.empty()}
+dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource or SHALL refer to the containing resource {contained.where((('#'+id in (%resource.descendants().reference | %resource.descendants().as(canonical) | %resource.descendants().as(uri) | %resource.descendants().as(url))) or descendants().where(reference = '#').exists() or descendants().where(as(canonical) = '#').exists() or descendants().where(as(canonical) = '#').exists()).not()).trace('unmatched', id).empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-5:If a resource is contained in another resource, it SHALL NOT have a security label {contained.meta.security.empty()}dom-6:A resource should have narrative for robust management {text.`div`.exists()}grp-1:Can only have members if group is "actual" {member.empty() or (actual = true)}</t>
+  </si>
+  <si>
+    <t>Group.id</t>
+  </si>
+  <si>
+    <t>Group.meta</t>
+  </si>
+  <si>
+    <t>Group.implicitRules</t>
+  </si>
+  <si>
+    <t>Group.language</t>
+  </si>
+  <si>
+    <t>Group.text</t>
+  </si>
+  <si>
+    <t>Group.contained</t>
+  </si>
+  <si>
+    <t>Group.extension</t>
+  </si>
+  <si>
+    <t>Group.modifierExtension</t>
+  </si>
+  <si>
+    <t>Group.identifier</t>
+  </si>
+  <si>
+    <t>Unique id</t>
+  </si>
+  <si>
+    <t>A unique business identifier for this group.</t>
+  </si>
+  <si>
+    <t>Allows the group to be referenced from external specifications.</t>
+  </si>
+  <si>
+    <t>Group.active</t>
+  </si>
+  <si>
+    <t>Whether this group's record is in active use</t>
+  </si>
+  <si>
+    <t>Indicates whether the record for the group is available for use or is merely being retained for historical purposes.</t>
+  </si>
+  <si>
+    <t>Need to be able to mark a group record as not to be used because it was created in error or is otherwise no longer available (e.g. a herd that no longer exists).</t>
+  </si>
+  <si>
+    <t>Group.type</t>
+  </si>
+  <si>
+    <t>person | animal | practitioner | device | medication | substance</t>
+  </si>
+  <si>
+    <t>Identifies the broad classification of the kind of resources the group includes.</t>
+  </si>
+  <si>
+    <t>Group members SHALL be of the appropriate resource type (Patient for person or animal; or Practitioner, Device, Medication or Substance for the other types.).</t>
+  </si>
+  <si>
+    <t>Identifies what type of resources the group is made up of.</t>
+  </si>
+  <si>
+    <t>person</t>
+  </si>
+  <si>
+    <t>Types of resources that are part of group.</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/ValueSet/group-type|4.0.1</t>
+  </si>
+  <si>
+    <t>Group.actual</t>
+  </si>
+  <si>
+    <t>Descriptive or actual</t>
+  </si>
+  <si>
+    <t>If true, indicates that the resource refers to a specific group of real individuals.  If false, the group defines a set of intended individuals.</t>
+  </si>
+  <si>
+    <t>There are use-cases for groups that define specific collections of individuals, and other groups that define "types" of intended individuals.  The requirements for both kinds of groups are similar, so we use a single resource, distinguished by this flag.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">grp-1
+</t>
+  </si>
+  <si>
+    <t>Group.code</t>
+  </si>
+  <si>
+    <t>Kind of Group members</t>
+  </si>
+  <si>
+    <t>Provides a specific type of resource the group includes; e.g. "cow", "syringe", etc.</t>
+  </si>
+  <si>
+    <t>This would generally be omitted for Person resources.</t>
+  </si>
+  <si>
+    <t>example</t>
+  </si>
+  <si>
+    <t>Kind of particular resource; e.g. cow, syringe, lake, etc.</t>
+  </si>
+  <si>
+    <t>Group.name</t>
+  </si>
+  <si>
+    <t>Label for Group</t>
+  </si>
+  <si>
+    <t>A label assigned to the group for human identification and communication.</t>
+  </si>
+  <si>
+    <t>Used to identify the group in human communication.</t>
+  </si>
+  <si>
+    <t>Group.quantity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unsignedInt
+</t>
+  </si>
+  <si>
+    <t>Number of members</t>
+  </si>
+  <si>
+    <t>A count of the number of resource instances that are part of the group.</t>
+  </si>
+  <si>
+    <t>Note that the quantity may be less than the number of members if some of the members are not active.</t>
+  </si>
+  <si>
+    <t>Group size is a common defining characteristic.</t>
+  </si>
+  <si>
+    <t>Group.managingEntity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reference(Organization|RelatedPerson|Practitioner|PractitionerRole)
+</t>
+  </si>
+  <si>
+    <t>Entity that is the custodian of the Group's definition</t>
+  </si>
+  <si>
+    <t>Entity responsible for defining and maintaining Group characteristics and/or registered members.</t>
+  </si>
+  <si>
+    <t>This does not strictly align with ownership of a herd or flock, but may suffice to represent that relationship in simple cases. More complex cases will require an extension.</t>
+  </si>
+  <si>
+    <t>Group.characteristic</t>
+  </si>
+  <si>
+    <t>Include / Exclude group members by Trait</t>
+  </si>
+  <si>
+    <t>Identifies traits whose presence r absence is shared by members of the group.</t>
+  </si>
+  <si>
+    <t>All the identified characteristics must be true for an entity to a member of the group.</t>
+  </si>
+  <si>
+    <t>Needs to be a generic mechanism for identifying what individuals can be part of a group.</t>
+  </si>
+  <si>
+    <t>Group.characteristic.id</t>
+  </si>
+  <si>
+    <t>Group.characteristic.extension</t>
+  </si>
+  <si>
+    <t>Group.characteristic.modifierExtension</t>
+  </si>
+  <si>
+    <t>Group.characteristic.code</t>
+  </si>
+  <si>
+    <t>Kind of characteristic</t>
+  </si>
+  <si>
+    <t>A code that identifies the kind of trait being asserted.</t>
+  </si>
+  <si>
+    <t>Need a formal way of identifying the characteristic being described.</t>
+  </si>
+  <si>
+    <t>List of characteristics used to describe group members; e.g. gender, age, owner, location, etc.</t>
+  </si>
+  <si>
+    <t>Group.characteristic.value[x]</t>
+  </si>
+  <si>
+    <t>CodeableConcept
+booleanQuantityRangeReference</t>
+  </si>
+  <si>
+    <t>Value held by characteristic</t>
+  </si>
+  <si>
+    <t>The value of the trait that holds (or does not hold - see 'exclude') for members of the group.</t>
+  </si>
+  <si>
+    <t>For Range, it means members of the group have a value that falls somewhere within the specified range.</t>
+  </si>
+  <si>
+    <t>The value of the characteristic is what determines group membership.</t>
+  </si>
+  <si>
+    <t>Value of descriptive member characteristic; e.g. red, male, pneumonia, Caucasian, etc.</t>
+  </si>
+  <si>
+    <t>Group.characteristic.exclude</t>
+  </si>
+  <si>
+    <t>Group includes or excludes</t>
+  </si>
+  <si>
+    <t>If true, indicates the characteristic is one that is NOT held by members of the group.</t>
+  </si>
+  <si>
+    <t>This is labeled as "Is Modifier" because applications cannot wrongly include excluded members as included or vice versa.</t>
+  </si>
+  <si>
+    <t>Sometimes group membership is determined by characteristics not possessed.</t>
+  </si>
+  <si>
+    <t>Group.characteristic.period</t>
+  </si>
+  <si>
+    <t>Period over which characteristic is tested</t>
+  </si>
+  <si>
+    <t>The period over which the characteristic is tested; e.g. the patient had an operation during the month of June.</t>
+  </si>
+  <si>
+    <t>Group.member</t>
+  </si>
+  <si>
+    <t>Who or what is in group</t>
+  </si>
+  <si>
+    <t>Identifies the resource instances that are members of the group.</t>
+  </si>
+  <si>
+    <t>Often the only thing of interest about a group is "who's in it".</t>
+  </si>
+  <si>
+    <t>Group.member.id</t>
+  </si>
+  <si>
+    <t>Group.member.extension</t>
+  </si>
+  <si>
+    <t>Group.member.modifierExtension</t>
+  </si>
+  <si>
+    <t>Group.member.entity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reference(Patient|Practitioner|PractitionerRole|Device|Medication|Substance|Group)
+</t>
+  </si>
+  <si>
+    <t>Reference to the group member</t>
+  </si>
+  <si>
+    <t>A reference to the entity that is a member of the group. Must be consistent with Group.type. If the entity is another group, then the type must be the same.</t>
+  </si>
+  <si>
+    <t>Group.member.period</t>
+  </si>
+  <si>
+    <t>Period member belonged to the group</t>
+  </si>
+  <si>
+    <t>The period that the member was in the group, if known.</t>
+  </si>
+  <si>
+    <t>Need to track who was in a group at a  particular time.</t>
+  </si>
+  <si>
+    <t>The member is in the group at this time</t>
+  </si>
+  <si>
+    <t>Group.member.inactive</t>
+  </si>
+  <si>
+    <t>If member is no longer in group</t>
+  </si>
+  <si>
+    <t>A flag to indicate that the member is no longer in the group, but previously may have been a member.</t>
+  </si>
+  <si>
+    <t>Sometimes you don't know when someone stopped being in a group, but not when.</t>
+  </si>
+  <si>
+    <t>Members are considered active unless explicitly specified otherwise</t>
   </si>
 </sst>
 </file>
@@ -1102,7 +1438,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B42"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -1272,6 +1608,168 @@
         <v>36</v>
       </c>
     </row>
+    <row r="22">
+      <c r="A22" t="s" s="1">
+        <v>0</v>
+      </c>
+      <c r="B22" t="s" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s" s="2">
+        <v>2</v>
+      </c>
+      <c r="B23" t="s" s="2">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s" s="2">
+        <v>4</v>
+      </c>
+      <c r="B24" t="s" s="2">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s" s="2">
+        <v>6</v>
+      </c>
+      <c r="B25" t="s" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="B26" t="s" s="2">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="B27" t="s" s="2">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="B28" t="s" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s" s="2">
+        <v>12</v>
+      </c>
+      <c r="B29" s="2"/>
+    </row>
+    <row r="30">
+      <c r="A30" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="B30" t="s" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s" s="2">
+        <v>15</v>
+      </c>
+      <c r="B31" t="s" s="2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s" s="2">
+        <v>17</v>
+      </c>
+      <c r="B32" t="s" s="2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="B33" t="s" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s" s="2">
+        <v>21</v>
+      </c>
+      <c r="B34" t="s" s="2">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s" s="2">
+        <v>23</v>
+      </c>
+      <c r="B35" s="2"/>
+    </row>
+    <row r="36">
+      <c r="A36" t="s" s="2">
+        <v>24</v>
+      </c>
+      <c r="B36" s="2"/>
+    </row>
+    <row r="37">
+      <c r="A37" t="s" s="2">
+        <v>25</v>
+      </c>
+      <c r="B37" t="s" s="2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s" s="2">
+        <v>27</v>
+      </c>
+      <c r="B38" t="s" s="2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s" s="2">
+        <v>29</v>
+      </c>
+      <c r="B39" t="s" s="2">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s" s="2">
+        <v>31</v>
+      </c>
+      <c r="B40" t="s" s="2">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s" s="2">
+        <v>33</v>
+      </c>
+      <c r="B41" t="s" s="2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="B42" t="s" s="2">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -1279,7 +1777,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AK46"/>
+  <dimension ref="A1:AK78"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -1288,7 +1786,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="12.13671875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="20.24609375" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="38.84375" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="38.84375" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="11.1328125" customWidth="true" bestFit="true" hidden="true"/>
@@ -1313,7 +1811,7 @@
     <col min="23" max="23" width="16.08984375" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="17.078125" customWidth="true" bestFit="true"/>
     <col min="25" max="25" width="16.3125" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="78.75390625" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="84.52734375" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="52.28125" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="5.69140625" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="19.73046875" customWidth="true" bestFit="true"/>
@@ -6191,6 +6689,3378 @@
         <v>93</v>
       </c>
     </row>
+    <row r="47">
+      <c r="A47" t="s" s="2">
+        <v>303</v>
+      </c>
+      <c r="B47" t="s" s="2">
+        <v>308</v>
+      </c>
+      <c r="C47" t="s" s="2">
+        <v>308</v>
+      </c>
+      <c r="D47" s="2"/>
+      <c r="E47" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="F47" s="2"/>
+      <c r="G47" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="H47" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="I47" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="J47" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="K47" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="L47" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="M47" t="s" s="2">
+        <v>310</v>
+      </c>
+      <c r="N47" t="s" s="2">
+        <v>311</v>
+      </c>
+      <c r="O47" t="s" s="2">
+        <v>312</v>
+      </c>
+      <c r="P47" s="2"/>
+      <c r="Q47" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="R47" s="2"/>
+      <c r="S47" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="T47" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="U47" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="V47" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="W47" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="X47" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Y47" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Z47" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AA47" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AB47" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AC47" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AD47" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AE47" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AF47" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AG47" t="s" s="2">
+        <v>308</v>
+      </c>
+      <c r="AH47" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AI47" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AJ47" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AK47" t="s" s="2">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s" s="2">
+        <v>303</v>
+      </c>
+      <c r="B48" t="s" s="2">
+        <v>314</v>
+      </c>
+      <c r="C48" t="s" s="2">
+        <v>314</v>
+      </c>
+      <c r="D48" s="2"/>
+      <c r="E48" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="F48" s="2"/>
+      <c r="G48" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="H48" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="I48" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="J48" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="K48" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="L48" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="M48" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="N48" t="s" s="2">
+        <v>85</v>
+      </c>
+      <c r="O48" t="s" s="2">
+        <v>86</v>
+      </c>
+      <c r="P48" s="2"/>
+      <c r="Q48" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="R48" s="2"/>
+      <c r="S48" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="T48" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="U48" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="V48" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="W48" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="X48" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Y48" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Z48" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AA48" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AB48" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AC48" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AD48" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AE48" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AF48" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AG48" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="AH48" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AI48" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="AJ48" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AK48" t="s" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s" s="2">
+        <v>303</v>
+      </c>
+      <c r="B49" t="s" s="2">
+        <v>315</v>
+      </c>
+      <c r="C49" t="s" s="2">
+        <v>315</v>
+      </c>
+      <c r="D49" s="2"/>
+      <c r="E49" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="F49" s="2"/>
+      <c r="G49" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="H49" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="I49" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="J49" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="K49" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="L49" t="s" s="2">
+        <v>89</v>
+      </c>
+      <c r="M49" t="s" s="2">
+        <v>90</v>
+      </c>
+      <c r="N49" t="s" s="2">
+        <v>91</v>
+      </c>
+      <c r="O49" s="2"/>
+      <c r="P49" s="2"/>
+      <c r="Q49" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="R49" s="2"/>
+      <c r="S49" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="T49" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="U49" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="V49" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="W49" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="X49" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Y49" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Z49" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AA49" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AB49" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AC49" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AD49" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AE49" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AF49" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AG49" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="AH49" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AI49" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="AJ49" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AK49" t="s" s="2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s" s="2">
+        <v>303</v>
+      </c>
+      <c r="B50" t="s" s="2">
+        <v>316</v>
+      </c>
+      <c r="C50" t="s" s="2">
+        <v>316</v>
+      </c>
+      <c r="D50" s="2"/>
+      <c r="E50" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="F50" s="2"/>
+      <c r="G50" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="H50" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="I50" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="J50" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="K50" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="L50" t="s" s="2">
+        <v>95</v>
+      </c>
+      <c r="M50" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="N50" t="s" s="2">
+        <v>97</v>
+      </c>
+      <c r="O50" t="s" s="2">
+        <v>98</v>
+      </c>
+      <c r="P50" s="2"/>
+      <c r="Q50" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="R50" s="2"/>
+      <c r="S50" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="T50" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="U50" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="V50" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="W50" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="X50" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Y50" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Z50" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AA50" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AB50" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AC50" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AD50" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AE50" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AF50" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AG50" t="s" s="2">
+        <v>99</v>
+      </c>
+      <c r="AH50" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AI50" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="AJ50" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AK50" t="s" s="2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s" s="2">
+        <v>303</v>
+      </c>
+      <c r="B51" t="s" s="2">
+        <v>317</v>
+      </c>
+      <c r="C51" t="s" s="2">
+        <v>317</v>
+      </c>
+      <c r="D51" s="2"/>
+      <c r="E51" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="F51" s="2"/>
+      <c r="G51" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="H51" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="I51" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="J51" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="K51" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="L51" t="s" s="2">
+        <v>101</v>
+      </c>
+      <c r="M51" t="s" s="2">
+        <v>102</v>
+      </c>
+      <c r="N51" t="s" s="2">
+        <v>103</v>
+      </c>
+      <c r="O51" t="s" s="2">
+        <v>104</v>
+      </c>
+      <c r="P51" s="2"/>
+      <c r="Q51" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="R51" s="2"/>
+      <c r="S51" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="T51" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="U51" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="V51" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="W51" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="X51" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Y51" t="s" s="2">
+        <v>105</v>
+      </c>
+      <c r="Z51" t="s" s="2">
+        <v>106</v>
+      </c>
+      <c r="AA51" t="s" s="2">
+        <v>107</v>
+      </c>
+      <c r="AB51" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AC51" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AD51" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AE51" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AF51" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AG51" t="s" s="2">
+        <v>108</v>
+      </c>
+      <c r="AH51" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AI51" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="AJ51" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AK51" t="s" s="2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s" s="2">
+        <v>303</v>
+      </c>
+      <c r="B52" t="s" s="2">
+        <v>318</v>
+      </c>
+      <c r="C52" t="s" s="2">
+        <v>318</v>
+      </c>
+      <c r="D52" s="2"/>
+      <c r="E52" t="s" s="2">
+        <v>110</v>
+      </c>
+      <c r="F52" s="2"/>
+      <c r="G52" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="H52" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="I52" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="J52" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="K52" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="L52" t="s" s="2">
+        <v>111</v>
+      </c>
+      <c r="M52" t="s" s="2">
+        <v>112</v>
+      </c>
+      <c r="N52" t="s" s="2">
+        <v>113</v>
+      </c>
+      <c r="O52" t="s" s="2">
+        <v>114</v>
+      </c>
+      <c r="P52" s="2"/>
+      <c r="Q52" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="R52" s="2"/>
+      <c r="S52" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="T52" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="U52" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="V52" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="W52" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="X52" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Y52" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Z52" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AA52" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AB52" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AC52" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AD52" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AE52" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AF52" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AG52" t="s" s="2">
+        <v>115</v>
+      </c>
+      <c r="AH52" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AI52" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="AJ52" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AK52" t="s" s="2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s" s="2">
+        <v>303</v>
+      </c>
+      <c r="B53" t="s" s="2">
+        <v>319</v>
+      </c>
+      <c r="C53" t="s" s="2">
+        <v>319</v>
+      </c>
+      <c r="D53" s="2"/>
+      <c r="E53" t="s" s="2">
+        <v>117</v>
+      </c>
+      <c r="F53" s="2"/>
+      <c r="G53" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="H53" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="I53" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="J53" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="K53" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="L53" t="s" s="2">
+        <v>118</v>
+      </c>
+      <c r="M53" t="s" s="2">
+        <v>119</v>
+      </c>
+      <c r="N53" t="s" s="2">
+        <v>120</v>
+      </c>
+      <c r="O53" t="s" s="2">
+        <v>121</v>
+      </c>
+      <c r="P53" s="2"/>
+      <c r="Q53" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="R53" s="2"/>
+      <c r="S53" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="T53" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="U53" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="V53" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="W53" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="X53" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Y53" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Z53" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AA53" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AB53" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AC53" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AD53" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AE53" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AF53" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AG53" t="s" s="2">
+        <v>122</v>
+      </c>
+      <c r="AH53" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AI53" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AJ53" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AK53" t="s" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s" s="2">
+        <v>303</v>
+      </c>
+      <c r="B54" t="s" s="2">
+        <v>320</v>
+      </c>
+      <c r="C54" t="s" s="2">
+        <v>320</v>
+      </c>
+      <c r="D54" s="2"/>
+      <c r="E54" t="s" s="2">
+        <v>124</v>
+      </c>
+      <c r="F54" s="2"/>
+      <c r="G54" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="H54" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="I54" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="J54" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="K54" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="L54" t="s" s="2">
+        <v>125</v>
+      </c>
+      <c r="M54" t="s" s="2">
+        <v>126</v>
+      </c>
+      <c r="N54" t="s" s="2">
+        <v>127</v>
+      </c>
+      <c r="O54" t="s" s="2">
+        <v>128</v>
+      </c>
+      <c r="P54" s="2"/>
+      <c r="Q54" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="R54" s="2"/>
+      <c r="S54" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="T54" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="U54" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="V54" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="W54" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="X54" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Y54" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Z54" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AA54" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AB54" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AC54" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AD54" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AE54" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AF54" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AG54" t="s" s="2">
+        <v>129</v>
+      </c>
+      <c r="AH54" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AI54" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AJ54" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AK54" t="s" s="2">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s" s="2">
+        <v>303</v>
+      </c>
+      <c r="B55" t="s" s="2">
+        <v>321</v>
+      </c>
+      <c r="C55" t="s" s="2">
+        <v>321</v>
+      </c>
+      <c r="D55" s="2"/>
+      <c r="E55" t="s" s="2">
+        <v>124</v>
+      </c>
+      <c r="F55" s="2"/>
+      <c r="G55" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="H55" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="I55" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="J55" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="K55" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="L55" t="s" s="2">
+        <v>125</v>
+      </c>
+      <c r="M55" t="s" s="2">
+        <v>132</v>
+      </c>
+      <c r="N55" t="s" s="2">
+        <v>133</v>
+      </c>
+      <c r="O55" t="s" s="2">
+        <v>128</v>
+      </c>
+      <c r="P55" t="s" s="2">
+        <v>134</v>
+      </c>
+      <c r="Q55" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="R55" s="2"/>
+      <c r="S55" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="T55" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="U55" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="V55" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="W55" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="X55" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Y55" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Z55" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AA55" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AB55" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AC55" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AD55" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AE55" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AF55" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AG55" t="s" s="2">
+        <v>135</v>
+      </c>
+      <c r="AH55" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AI55" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AJ55" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AK55" t="s" s="2">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s" s="2">
+        <v>303</v>
+      </c>
+      <c r="B56" t="s" s="2">
+        <v>322</v>
+      </c>
+      <c r="C56" t="s" s="2">
+        <v>322</v>
+      </c>
+      <c r="D56" s="2"/>
+      <c r="E56" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="F56" s="2"/>
+      <c r="G56" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="H56" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="I56" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="J56" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="K56" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="L56" t="s" s="2">
+        <v>137</v>
+      </c>
+      <c r="M56" t="s" s="2">
+        <v>323</v>
+      </c>
+      <c r="N56" t="s" s="2">
+        <v>324</v>
+      </c>
+      <c r="O56" s="2"/>
+      <c r="P56" t="s" s="2">
+        <v>325</v>
+      </c>
+      <c r="Q56" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="R56" s="2"/>
+      <c r="S56" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="T56" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="U56" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="V56" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="W56" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="X56" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Y56" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Z56" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AA56" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AB56" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AC56" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AD56" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AE56" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AF56" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AG56" t="s" s="2">
+        <v>322</v>
+      </c>
+      <c r="AH56" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AI56" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AJ56" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AK56" t="s" s="2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s" s="2">
+        <v>303</v>
+      </c>
+      <c r="B57" t="s" s="2">
+        <v>326</v>
+      </c>
+      <c r="C57" t="s" s="2">
+        <v>326</v>
+      </c>
+      <c r="D57" s="2"/>
+      <c r="E57" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="F57" s="2"/>
+      <c r="G57" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="H57" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="I57" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="J57" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="K57" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="L57" t="s" s="2">
+        <v>142</v>
+      </c>
+      <c r="M57" t="s" s="2">
+        <v>327</v>
+      </c>
+      <c r="N57" t="s" s="2">
+        <v>328</v>
+      </c>
+      <c r="O57" s="2"/>
+      <c r="P57" t="s" s="2">
+        <v>329</v>
+      </c>
+      <c r="Q57" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="R57" t="s" s="2">
+        <v>147</v>
+      </c>
+      <c r="S57" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="T57" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="U57" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="V57" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="W57" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="X57" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Y57" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Z57" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AA57" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AB57" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AC57" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AD57" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AE57" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AF57" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AG57" t="s" s="2">
+        <v>326</v>
+      </c>
+      <c r="AH57" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AI57" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="AJ57" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AK57" t="s" s="2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s" s="2">
+        <v>303</v>
+      </c>
+      <c r="B58" t="s" s="2">
+        <v>330</v>
+      </c>
+      <c r="C58" t="s" s="2">
+        <v>330</v>
+      </c>
+      <c r="D58" s="2"/>
+      <c r="E58" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="F58" s="2"/>
+      <c r="G58" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="H58" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="I58" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="J58" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="K58" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="L58" t="s" s="2">
+        <v>101</v>
+      </c>
+      <c r="M58" t="s" s="2">
+        <v>331</v>
+      </c>
+      <c r="N58" t="s" s="2">
+        <v>332</v>
+      </c>
+      <c r="O58" t="s" s="2">
+        <v>333</v>
+      </c>
+      <c r="P58" t="s" s="2">
+        <v>334</v>
+      </c>
+      <c r="Q58" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="R58" s="2"/>
+      <c r="S58" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="T58" t="s" s="2">
+        <v>335</v>
+      </c>
+      <c r="U58" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="V58" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="W58" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="X58" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Y58" t="s" s="2">
+        <v>165</v>
+      </c>
+      <c r="Z58" t="s" s="2">
+        <v>336</v>
+      </c>
+      <c r="AA58" t="s" s="2">
+        <v>337</v>
+      </c>
+      <c r="AB58" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AC58" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AD58" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AE58" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AF58" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AG58" t="s" s="2">
+        <v>330</v>
+      </c>
+      <c r="AH58" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="AI58" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="AJ58" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AK58" t="s" s="2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s" s="2">
+        <v>303</v>
+      </c>
+      <c r="B59" t="s" s="2">
+        <v>338</v>
+      </c>
+      <c r="C59" t="s" s="2">
+        <v>338</v>
+      </c>
+      <c r="D59" s="2"/>
+      <c r="E59" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="F59" s="2"/>
+      <c r="G59" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="H59" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="I59" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="J59" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="K59" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="L59" t="s" s="2">
+        <v>142</v>
+      </c>
+      <c r="M59" t="s" s="2">
+        <v>339</v>
+      </c>
+      <c r="N59" t="s" s="2">
+        <v>340</v>
+      </c>
+      <c r="O59" s="2"/>
+      <c r="P59" t="s" s="2">
+        <v>341</v>
+      </c>
+      <c r="Q59" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="R59" s="2"/>
+      <c r="S59" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="T59" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="U59" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="V59" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="W59" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="X59" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Y59" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Z59" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AA59" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AB59" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AC59" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AD59" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AE59" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AF59" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AG59" t="s" s="2">
+        <v>338</v>
+      </c>
+      <c r="AH59" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="AI59" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="AJ59" t="s" s="2">
+        <v>342</v>
+      </c>
+      <c r="AK59" t="s" s="2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s" s="2">
+        <v>303</v>
+      </c>
+      <c r="B60" t="s" s="2">
+        <v>343</v>
+      </c>
+      <c r="C60" t="s" s="2">
+        <v>343</v>
+      </c>
+      <c r="D60" s="2"/>
+      <c r="E60" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="F60" s="2"/>
+      <c r="G60" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="H60" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="I60" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="J60" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="K60" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="L60" t="s" s="2">
+        <v>187</v>
+      </c>
+      <c r="M60" t="s" s="2">
+        <v>344</v>
+      </c>
+      <c r="N60" t="s" s="2">
+        <v>345</v>
+      </c>
+      <c r="O60" t="s" s="2">
+        <v>346</v>
+      </c>
+      <c r="P60" s="2"/>
+      <c r="Q60" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="R60" s="2"/>
+      <c r="S60" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="T60" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="U60" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="V60" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="W60" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="X60" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Y60" t="s" s="2">
+        <v>347</v>
+      </c>
+      <c r="Z60" t="s" s="2">
+        <v>348</v>
+      </c>
+      <c r="AA60" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AB60" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AC60" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AD60" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AE60" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AF60" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AG60" t="s" s="2">
+        <v>343</v>
+      </c>
+      <c r="AH60" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AI60" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="AJ60" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AK60" t="s" s="2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="s" s="2">
+        <v>303</v>
+      </c>
+      <c r="B61" t="s" s="2">
+        <v>349</v>
+      </c>
+      <c r="C61" t="s" s="2">
+        <v>349</v>
+      </c>
+      <c r="D61" s="2"/>
+      <c r="E61" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="F61" s="2"/>
+      <c r="G61" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="H61" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="I61" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="J61" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="K61" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="L61" t="s" s="2">
+        <v>214</v>
+      </c>
+      <c r="M61" t="s" s="2">
+        <v>350</v>
+      </c>
+      <c r="N61" t="s" s="2">
+        <v>351</v>
+      </c>
+      <c r="O61" s="2"/>
+      <c r="P61" t="s" s="2">
+        <v>352</v>
+      </c>
+      <c r="Q61" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="R61" s="2"/>
+      <c r="S61" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="T61" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="U61" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="V61" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="W61" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="X61" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Y61" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Z61" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AA61" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AB61" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AC61" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AD61" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AE61" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AF61" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AG61" t="s" s="2">
+        <v>349</v>
+      </c>
+      <c r="AH61" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AI61" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="AJ61" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AK61" t="s" s="2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s" s="2">
+        <v>303</v>
+      </c>
+      <c r="B62" t="s" s="2">
+        <v>353</v>
+      </c>
+      <c r="C62" t="s" s="2">
+        <v>353</v>
+      </c>
+      <c r="D62" s="2"/>
+      <c r="E62" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="F62" s="2"/>
+      <c r="G62" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="H62" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="I62" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="J62" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="K62" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="L62" t="s" s="2">
+        <v>354</v>
+      </c>
+      <c r="M62" t="s" s="2">
+        <v>355</v>
+      </c>
+      <c r="N62" t="s" s="2">
+        <v>356</v>
+      </c>
+      <c r="O62" t="s" s="2">
+        <v>357</v>
+      </c>
+      <c r="P62" t="s" s="2">
+        <v>358</v>
+      </c>
+      <c r="Q62" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="R62" s="2"/>
+      <c r="S62" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="T62" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="U62" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="V62" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="W62" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="X62" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Y62" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Z62" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AA62" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AB62" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AC62" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AD62" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AE62" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AF62" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AG62" t="s" s="2">
+        <v>353</v>
+      </c>
+      <c r="AH62" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AI62" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="AJ62" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AK62" t="s" s="2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="s" s="2">
+        <v>303</v>
+      </c>
+      <c r="B63" t="s" s="2">
+        <v>359</v>
+      </c>
+      <c r="C63" t="s" s="2">
+        <v>359</v>
+      </c>
+      <c r="D63" s="2"/>
+      <c r="E63" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="F63" s="2"/>
+      <c r="G63" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="H63" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="I63" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="J63" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="K63" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="L63" t="s" s="2">
+        <v>360</v>
+      </c>
+      <c r="M63" t="s" s="2">
+        <v>361</v>
+      </c>
+      <c r="N63" t="s" s="2">
+        <v>362</v>
+      </c>
+      <c r="O63" t="s" s="2">
+        <v>363</v>
+      </c>
+      <c r="P63" s="2"/>
+      <c r="Q63" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="R63" s="2"/>
+      <c r="S63" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="T63" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="U63" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="V63" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="W63" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="X63" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Y63" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Z63" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AA63" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AB63" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AC63" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AD63" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AE63" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AF63" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AG63" t="s" s="2">
+        <v>359</v>
+      </c>
+      <c r="AH63" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AI63" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="AJ63" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AK63" t="s" s="2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="s" s="2">
+        <v>303</v>
+      </c>
+      <c r="B64" t="s" s="2">
+        <v>364</v>
+      </c>
+      <c r="C64" t="s" s="2">
+        <v>364</v>
+      </c>
+      <c r="D64" s="2"/>
+      <c r="E64" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="F64" s="2"/>
+      <c r="G64" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="H64" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="I64" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="J64" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="K64" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="L64" t="s" s="2">
+        <v>207</v>
+      </c>
+      <c r="M64" t="s" s="2">
+        <v>365</v>
+      </c>
+      <c r="N64" t="s" s="2">
+        <v>366</v>
+      </c>
+      <c r="O64" t="s" s="2">
+        <v>367</v>
+      </c>
+      <c r="P64" t="s" s="2">
+        <v>368</v>
+      </c>
+      <c r="Q64" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="R64" s="2"/>
+      <c r="S64" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="T64" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="U64" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="V64" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="W64" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="X64" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Y64" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Z64" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AA64" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AB64" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AC64" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AD64" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AE64" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AF64" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AG64" t="s" s="2">
+        <v>364</v>
+      </c>
+      <c r="AH64" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AI64" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AJ64" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AK64" t="s" s="2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s" s="2">
+        <v>303</v>
+      </c>
+      <c r="B65" t="s" s="2">
+        <v>369</v>
+      </c>
+      <c r="C65" t="s" s="2">
+        <v>369</v>
+      </c>
+      <c r="D65" s="2"/>
+      <c r="E65" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="F65" s="2"/>
+      <c r="G65" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="H65" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="I65" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="J65" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="K65" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="L65" t="s" s="2">
+        <v>214</v>
+      </c>
+      <c r="M65" t="s" s="2">
+        <v>215</v>
+      </c>
+      <c r="N65" t="s" s="2">
+        <v>216</v>
+      </c>
+      <c r="O65" s="2"/>
+      <c r="P65" s="2"/>
+      <c r="Q65" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="R65" s="2"/>
+      <c r="S65" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="T65" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="U65" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="V65" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="W65" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="X65" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Y65" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Z65" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AA65" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AB65" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AC65" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AD65" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AE65" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AF65" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AG65" t="s" s="2">
+        <v>217</v>
+      </c>
+      <c r="AH65" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AI65" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="AJ65" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AK65" t="s" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s" s="2">
+        <v>303</v>
+      </c>
+      <c r="B66" t="s" s="2">
+        <v>370</v>
+      </c>
+      <c r="C66" t="s" s="2">
+        <v>370</v>
+      </c>
+      <c r="D66" s="2"/>
+      <c r="E66" t="s" s="2">
+        <v>124</v>
+      </c>
+      <c r="F66" s="2"/>
+      <c r="G66" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="H66" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="I66" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="J66" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="K66" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="L66" t="s" s="2">
+        <v>125</v>
+      </c>
+      <c r="M66" t="s" s="2">
+        <v>126</v>
+      </c>
+      <c r="N66" t="s" s="2">
+        <v>219</v>
+      </c>
+      <c r="O66" t="s" s="2">
+        <v>128</v>
+      </c>
+      <c r="P66" s="2"/>
+      <c r="Q66" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="R66" s="2"/>
+      <c r="S66" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="T66" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="U66" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="V66" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="W66" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="X66" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Y66" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Z66" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AA66" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AB66" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AC66" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AD66" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AE66" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AF66" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AG66" t="s" s="2">
+        <v>220</v>
+      </c>
+      <c r="AH66" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AI66" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AJ66" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AK66" t="s" s="2">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="s" s="2">
+        <v>303</v>
+      </c>
+      <c r="B67" t="s" s="2">
+        <v>371</v>
+      </c>
+      <c r="C67" t="s" s="2">
+        <v>371</v>
+      </c>
+      <c r="D67" s="2"/>
+      <c r="E67" t="s" s="2">
+        <v>222</v>
+      </c>
+      <c r="F67" s="2"/>
+      <c r="G67" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="H67" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="I67" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="J67" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="K67" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="L67" t="s" s="2">
+        <v>125</v>
+      </c>
+      <c r="M67" t="s" s="2">
+        <v>223</v>
+      </c>
+      <c r="N67" t="s" s="2">
+        <v>224</v>
+      </c>
+      <c r="O67" t="s" s="2">
+        <v>128</v>
+      </c>
+      <c r="P67" t="s" s="2">
+        <v>134</v>
+      </c>
+      <c r="Q67" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="R67" s="2"/>
+      <c r="S67" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="T67" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="U67" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="V67" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="W67" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="X67" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Y67" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Z67" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AA67" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AB67" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AC67" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AD67" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AE67" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AF67" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AG67" t="s" s="2">
+        <v>225</v>
+      </c>
+      <c r="AH67" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AI67" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AJ67" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AK67" t="s" s="2">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="s" s="2">
+        <v>303</v>
+      </c>
+      <c r="B68" t="s" s="2">
+        <v>372</v>
+      </c>
+      <c r="C68" t="s" s="2">
+        <v>372</v>
+      </c>
+      <c r="D68" s="2"/>
+      <c r="E68" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="F68" s="2"/>
+      <c r="G68" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="H68" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="I68" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="J68" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="K68" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="L68" t="s" s="2">
+        <v>187</v>
+      </c>
+      <c r="M68" t="s" s="2">
+        <v>373</v>
+      </c>
+      <c r="N68" t="s" s="2">
+        <v>374</v>
+      </c>
+      <c r="O68" s="2"/>
+      <c r="P68" t="s" s="2">
+        <v>375</v>
+      </c>
+      <c r="Q68" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="R68" s="2"/>
+      <c r="S68" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="T68" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="U68" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="V68" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="W68" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="X68" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Y68" t="s" s="2">
+        <v>347</v>
+      </c>
+      <c r="Z68" t="s" s="2">
+        <v>376</v>
+      </c>
+      <c r="AA68" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AB68" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AC68" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AD68" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AE68" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AF68" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AG68" t="s" s="2">
+        <v>372</v>
+      </c>
+      <c r="AH68" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="AI68" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="AJ68" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AK68" t="s" s="2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="s" s="2">
+        <v>303</v>
+      </c>
+      <c r="B69" t="s" s="2">
+        <v>377</v>
+      </c>
+      <c r="C69" t="s" s="2">
+        <v>377</v>
+      </c>
+      <c r="D69" s="2"/>
+      <c r="E69" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="F69" s="2"/>
+      <c r="G69" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="H69" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="I69" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="J69" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="K69" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="L69" t="s" s="2">
+        <v>378</v>
+      </c>
+      <c r="M69" t="s" s="2">
+        <v>379</v>
+      </c>
+      <c r="N69" t="s" s="2">
+        <v>380</v>
+      </c>
+      <c r="O69" t="s" s="2">
+        <v>381</v>
+      </c>
+      <c r="P69" t="s" s="2">
+        <v>382</v>
+      </c>
+      <c r="Q69" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="R69" s="2"/>
+      <c r="S69" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="T69" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="U69" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="V69" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="W69" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="X69" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Y69" t="s" s="2">
+        <v>347</v>
+      </c>
+      <c r="Z69" t="s" s="2">
+        <v>383</v>
+      </c>
+      <c r="AA69" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AB69" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AC69" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AD69" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AE69" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AF69" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AG69" t="s" s="2">
+        <v>377</v>
+      </c>
+      <c r="AH69" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="AI69" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="AJ69" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AK69" t="s" s="2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="s" s="2">
+        <v>303</v>
+      </c>
+      <c r="B70" t="s" s="2">
+        <v>384</v>
+      </c>
+      <c r="C70" t="s" s="2">
+        <v>384</v>
+      </c>
+      <c r="D70" s="2"/>
+      <c r="E70" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="F70" s="2"/>
+      <c r="G70" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="H70" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="I70" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="J70" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="K70" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="L70" t="s" s="2">
+        <v>142</v>
+      </c>
+      <c r="M70" t="s" s="2">
+        <v>385</v>
+      </c>
+      <c r="N70" t="s" s="2">
+        <v>386</v>
+      </c>
+      <c r="O70" t="s" s="2">
+        <v>387</v>
+      </c>
+      <c r="P70" t="s" s="2">
+        <v>388</v>
+      </c>
+      <c r="Q70" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="R70" s="2"/>
+      <c r="S70" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="T70" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="U70" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="V70" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="W70" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="X70" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Y70" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Z70" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AA70" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AB70" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AC70" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AD70" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AE70" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AF70" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AG70" t="s" s="2">
+        <v>384</v>
+      </c>
+      <c r="AH70" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="AI70" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="AJ70" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AK70" t="s" s="2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="s" s="2">
+        <v>303</v>
+      </c>
+      <c r="B71" t="s" s="2">
+        <v>389</v>
+      </c>
+      <c r="C71" t="s" s="2">
+        <v>389</v>
+      </c>
+      <c r="D71" s="2"/>
+      <c r="E71" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="F71" s="2"/>
+      <c r="G71" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="H71" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="I71" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="J71" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="K71" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="L71" t="s" s="2">
+        <v>254</v>
+      </c>
+      <c r="M71" t="s" s="2">
+        <v>390</v>
+      </c>
+      <c r="N71" t="s" s="2">
+        <v>391</v>
+      </c>
+      <c r="O71" s="2"/>
+      <c r="P71" s="2"/>
+      <c r="Q71" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="R71" s="2"/>
+      <c r="S71" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="T71" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="U71" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="V71" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="W71" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="X71" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Y71" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Z71" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AA71" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AB71" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AC71" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AD71" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AE71" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AF71" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AG71" t="s" s="2">
+        <v>389</v>
+      </c>
+      <c r="AH71" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AI71" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="AJ71" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AK71" t="s" s="2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="s" s="2">
+        <v>303</v>
+      </c>
+      <c r="B72" t="s" s="2">
+        <v>392</v>
+      </c>
+      <c r="C72" t="s" s="2">
+        <v>392</v>
+      </c>
+      <c r="D72" s="2"/>
+      <c r="E72" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="F72" s="2"/>
+      <c r="G72" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="H72" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="I72" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="J72" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="K72" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="L72" t="s" s="2">
+        <v>207</v>
+      </c>
+      <c r="M72" t="s" s="2">
+        <v>393</v>
+      </c>
+      <c r="N72" t="s" s="2">
+        <v>394</v>
+      </c>
+      <c r="O72" s="2"/>
+      <c r="P72" t="s" s="2">
+        <v>395</v>
+      </c>
+      <c r="Q72" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="R72" s="2"/>
+      <c r="S72" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="T72" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="U72" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="V72" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="W72" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="X72" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Y72" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Z72" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AA72" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AB72" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AC72" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AD72" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AE72" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AF72" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AG72" t="s" s="2">
+        <v>392</v>
+      </c>
+      <c r="AH72" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AI72" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AJ72" t="s" s="2">
+        <v>342</v>
+      </c>
+      <c r="AK72" t="s" s="2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="s" s="2">
+        <v>303</v>
+      </c>
+      <c r="B73" t="s" s="2">
+        <v>396</v>
+      </c>
+      <c r="C73" t="s" s="2">
+        <v>396</v>
+      </c>
+      <c r="D73" s="2"/>
+      <c r="E73" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="F73" s="2"/>
+      <c r="G73" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="H73" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="I73" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="J73" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="K73" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="L73" t="s" s="2">
+        <v>214</v>
+      </c>
+      <c r="M73" t="s" s="2">
+        <v>215</v>
+      </c>
+      <c r="N73" t="s" s="2">
+        <v>216</v>
+      </c>
+      <c r="O73" s="2"/>
+      <c r="P73" s="2"/>
+      <c r="Q73" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="R73" s="2"/>
+      <c r="S73" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="T73" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="U73" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="V73" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="W73" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="X73" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Y73" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Z73" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AA73" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AB73" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AC73" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AD73" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AE73" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AF73" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AG73" t="s" s="2">
+        <v>217</v>
+      </c>
+      <c r="AH73" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AI73" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="AJ73" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AK73" t="s" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="s" s="2">
+        <v>303</v>
+      </c>
+      <c r="B74" t="s" s="2">
+        <v>397</v>
+      </c>
+      <c r="C74" t="s" s="2">
+        <v>397</v>
+      </c>
+      <c r="D74" s="2"/>
+      <c r="E74" t="s" s="2">
+        <v>124</v>
+      </c>
+      <c r="F74" s="2"/>
+      <c r="G74" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="H74" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="I74" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="J74" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="K74" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="L74" t="s" s="2">
+        <v>125</v>
+      </c>
+      <c r="M74" t="s" s="2">
+        <v>126</v>
+      </c>
+      <c r="N74" t="s" s="2">
+        <v>219</v>
+      </c>
+      <c r="O74" t="s" s="2">
+        <v>128</v>
+      </c>
+      <c r="P74" s="2"/>
+      <c r="Q74" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="R74" s="2"/>
+      <c r="S74" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="T74" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="U74" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="V74" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="W74" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="X74" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Y74" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Z74" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AA74" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AB74" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AC74" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AD74" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AE74" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AF74" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AG74" t="s" s="2">
+        <v>220</v>
+      </c>
+      <c r="AH74" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AI74" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AJ74" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AK74" t="s" s="2">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="s" s="2">
+        <v>303</v>
+      </c>
+      <c r="B75" t="s" s="2">
+        <v>398</v>
+      </c>
+      <c r="C75" t="s" s="2">
+        <v>398</v>
+      </c>
+      <c r="D75" s="2"/>
+      <c r="E75" t="s" s="2">
+        <v>222</v>
+      </c>
+      <c r="F75" s="2"/>
+      <c r="G75" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="H75" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="I75" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="J75" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="K75" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="L75" t="s" s="2">
+        <v>125</v>
+      </c>
+      <c r="M75" t="s" s="2">
+        <v>223</v>
+      </c>
+      <c r="N75" t="s" s="2">
+        <v>224</v>
+      </c>
+      <c r="O75" t="s" s="2">
+        <v>128</v>
+      </c>
+      <c r="P75" t="s" s="2">
+        <v>134</v>
+      </c>
+      <c r="Q75" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="R75" s="2"/>
+      <c r="S75" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="T75" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="U75" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="V75" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="W75" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="X75" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Y75" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Z75" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AA75" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AB75" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AC75" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AD75" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AE75" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AF75" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AG75" t="s" s="2">
+        <v>225</v>
+      </c>
+      <c r="AH75" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AI75" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AJ75" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AK75" t="s" s="2">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="s" s="2">
+        <v>303</v>
+      </c>
+      <c r="B76" t="s" s="2">
+        <v>399</v>
+      </c>
+      <c r="C76" t="s" s="2">
+        <v>399</v>
+      </c>
+      <c r="D76" s="2"/>
+      <c r="E76" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="F76" s="2"/>
+      <c r="G76" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="H76" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="I76" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="J76" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="K76" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="L76" t="s" s="2">
+        <v>400</v>
+      </c>
+      <c r="M76" t="s" s="2">
+        <v>401</v>
+      </c>
+      <c r="N76" t="s" s="2">
+        <v>402</v>
+      </c>
+      <c r="O76" s="2"/>
+      <c r="P76" s="2"/>
+      <c r="Q76" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="R76" s="2"/>
+      <c r="S76" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="T76" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="U76" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="V76" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="W76" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="X76" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Y76" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Z76" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AA76" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AB76" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AC76" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AD76" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AE76" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AF76" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AG76" t="s" s="2">
+        <v>399</v>
+      </c>
+      <c r="AH76" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="AI76" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="AJ76" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AK76" t="s" s="2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="s" s="2">
+        <v>303</v>
+      </c>
+      <c r="B77" t="s" s="2">
+        <v>403</v>
+      </c>
+      <c r="C77" t="s" s="2">
+        <v>403</v>
+      </c>
+      <c r="D77" s="2"/>
+      <c r="E77" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="F77" s="2"/>
+      <c r="G77" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="H77" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="I77" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="J77" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="K77" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="L77" t="s" s="2">
+        <v>254</v>
+      </c>
+      <c r="M77" t="s" s="2">
+        <v>404</v>
+      </c>
+      <c r="N77" t="s" s="2">
+        <v>405</v>
+      </c>
+      <c r="O77" s="2"/>
+      <c r="P77" t="s" s="2">
+        <v>406</v>
+      </c>
+      <c r="Q77" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="R77" t="s" s="2">
+        <v>407</v>
+      </c>
+      <c r="S77" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="T77" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="U77" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="V77" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="W77" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="X77" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Y77" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Z77" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AA77" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AB77" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AC77" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AD77" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AE77" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AF77" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AG77" t="s" s="2">
+        <v>403</v>
+      </c>
+      <c r="AH77" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AI77" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="AJ77" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AK77" t="s" s="2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="s" s="2">
+        <v>303</v>
+      </c>
+      <c r="B78" t="s" s="2">
+        <v>408</v>
+      </c>
+      <c r="C78" t="s" s="2">
+        <v>408</v>
+      </c>
+      <c r="D78" s="2"/>
+      <c r="E78" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="F78" s="2"/>
+      <c r="G78" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="H78" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="I78" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="J78" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="K78" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="L78" t="s" s="2">
+        <v>142</v>
+      </c>
+      <c r="M78" t="s" s="2">
+        <v>409</v>
+      </c>
+      <c r="N78" t="s" s="2">
+        <v>410</v>
+      </c>
+      <c r="O78" s="2"/>
+      <c r="P78" t="s" s="2">
+        <v>411</v>
+      </c>
+      <c r="Q78" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="R78" t="s" s="2">
+        <v>412</v>
+      </c>
+      <c r="S78" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="T78" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="U78" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="V78" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="W78" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="X78" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Y78" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Z78" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AA78" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AB78" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AC78" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AD78" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AE78" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AF78" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AG78" t="s" s="2">
+        <v>408</v>
+      </c>
+      <c r="AH78" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AI78" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="AJ78" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AK78" t="s" s="2">
+        <v>93</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>